<commit_message>
commit changes on exporting all reports
</commit_message>
<xml_diff>
--- a/library/export_pr.xlsx
+++ b/library/export_pr.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fas2020\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fas\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A68999-E07A-45AC-9412-C5F00A7E43FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23055" windowHeight="13740"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$43</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,8 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,13 +110,13 @@
     <t>ARIEL O. IGLESIA</t>
   </si>
   <si>
-    <t xml:space="preserve">PURCHASE ReEQUEST </t>
+    <t xml:space="preserve">PURCHASE REQUEST </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
@@ -865,39 +868,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="10" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="10" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="E1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="57"/>
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
@@ -905,7 +908,7 @@
       <c r="E3" s="57"/>
       <c r="F3" s="57"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
         <v>24</v>
       </c>
@@ -915,7 +918,7 @@
       <c r="E4" s="57"/>
       <c r="F4" s="57"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
       <c r="B5" s="58"/>
       <c r="C5" s="58"/>
@@ -923,7 +926,7 @@
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
     </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -937,7 +940,7 @@
       <c r="E6" s="59"/>
       <c r="F6" s="59"/>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -949,7 +952,7 @@
       </c>
       <c r="F7" s="55"/>
     </row>
-    <row r="8" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="50"/>
       <c r="B8" s="51"/>
       <c r="C8" s="9" t="s">
@@ -959,7 +962,7 @@
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="52" t="s">
         <v>7</v>
       </c>
@@ -979,7 +982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="53"/>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -987,7 +990,7 @@
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
@@ -995,7 +998,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1003,7 +1006,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1011,7 +1014,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1019,7 +1022,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1027,7 +1030,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -1035,7 +1038,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
@@ -1043,7 +1046,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
@@ -1051,7 +1054,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
@@ -1059,7 +1062,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
@@ -1067,7 +1070,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -1075,7 +1078,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -1083,7 +1086,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
@@ -1091,7 +1094,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -1099,7 +1102,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -1107,7 +1110,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
     </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -1115,7 +1118,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
@@ -1123,7 +1126,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -1131,7 +1134,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -1139,7 +1142,7 @@
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -1147,7 +1150,7 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
@@ -1155,7 +1158,7 @@
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -1163,7 +1166,7 @@
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
     </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -1171,7 +1174,7 @@
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -1179,7 +1182,7 @@
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -1187,12 +1190,9 @@
       <c r="E35" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="24">
-        <f>SUM(F11:F34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="24"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
         <v>14</v>
       </c>
@@ -1202,7 +1202,7 @@
       <c r="E36" s="39"/>
       <c r="F36" s="40"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37"/>
       <c r="B37" s="41"/>
       <c r="C37" s="41"/>
@@ -1210,7 +1210,7 @@
       <c r="E37" s="41"/>
       <c r="F37" s="42"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="37"/>
       <c r="B38" s="41"/>
       <c r="C38" s="41"/>
@@ -1218,7 +1218,7 @@
       <c r="E38" s="41"/>
       <c r="F38" s="42"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="38"/>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -1226,7 +1226,7 @@
       <c r="E39" s="31"/>
       <c r="F39" s="43"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="25"/>
       <c r="B40" s="44" t="s">
         <v>15</v>
@@ -1238,7 +1238,7 @@
       <c r="E40" s="45"/>
       <c r="F40" s="46"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>17</v>
       </c>
@@ -1248,7 +1248,7 @@
       <c r="E41" s="48"/>
       <c r="F41" s="49"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>18</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="E42" s="29"/>
       <c r="F42" s="30"/>
     </row>
-    <row r="43" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="27" t="s">
         <v>20</v>
       </c>
@@ -1304,6 +1304,6 @@
     <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="71" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>